<commit_message>
bug to be fix
</commit_message>
<xml_diff>
--- a/ClientA/Test_Data/demo1.xlsx
+++ b/ClientA/Test_Data/demo1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nelsonkct/Documents/Project/ClientA/Test_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D6F932A-F189-EE46-A03E-5EC429B5708E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B1B70A-02FF-344F-976D-361105745A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17140" xr2:uid="{95775AAB-8992-9242-9763-56A3C2ACD5AF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>id1</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>Rich</t>
+  </si>
+  <si>
+    <t>Dic</t>
+  </si>
+  <si>
+    <t>Eri</t>
   </si>
 </sst>
 </file>
@@ -410,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA6FB359-A218-2446-882E-1849929991AE}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,6 +466,20 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>111</v>
+      </c>
+      <c r="B4">
+        <v>222</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>